<commit_message>
mise à jour diag+début pop up
</commit_message>
<xml_diff>
--- a/Diagramme GANTT.xlsx
+++ b/Diagramme GANTT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MARY\Mirror\S6\CPO\Projet Escape Shark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MARY\Mirror\S6\CPO\escape-shark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA3BFDA-7530-4EDB-A3B9-42A30E6B37BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03603765-7E1F-45EB-AD0A-43116E055BB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E563E8D1-7FF8-4507-9344-36679DBFC1DA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>semaine 14</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>création du Gitlab</t>
+  </si>
+  <si>
+    <t>rajouter des pops-up d'information</t>
   </si>
 </sst>
 </file>
@@ -134,7 +137,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -157,11 +160,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -182,11 +207,16 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FB65A7-A251-4DF1-AD70-DADB90B3DB0E}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,7 +542,7 @@
     <col min="1" max="1" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -545,11 +575,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="10"/>
+      <c r="B2" s="9"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
@@ -560,12 +590,12 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="7"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -575,12 +605,11 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="9"/>
+        <v>19</v>
+      </c>
+      <c r="C4" s="8"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -590,123 +619,116 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="C5" s="8"/>
+      <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-    </row>
-    <row r="6" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="K5" s="10"/>
+      <c r="L5" s="11"/>
+    </row>
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="9"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-    </row>
-    <row r="7" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>14</v>
+      <c r="K6" s="10"/>
+      <c r="L6" s="11"/>
+    </row>
+    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="9"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="K7" s="10"/>
+      <c r="L7" s="11"/>
+    </row>
+    <row r="8" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="9"/>
+      <c r="G8" s="8"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-    </row>
-    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
+      <c r="K8" s="10"/>
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="9"/>
+      <c r="H9" s="8"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-    </row>
-    <row r="10" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="K9" s="10"/>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="9"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="5"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K10" s="10"/>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="8"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -719,7 +741,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -732,7 +754,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -745,7 +767,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>